<commit_message>
update some bug documentation data
</commit_message>
<xml_diff>
--- a/DesignAndExecution/Bugs PetStore.xlsx
+++ b/DesignAndExecution/Bugs PetStore.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\drago\OneDrive\Escritorio\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\drago\OneDrive\Escritorio\Punto Singular\Proyecto Plan de Pruebas\Pruebas Esploratorias\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEEA833B-4E3F-4A6E-A7A1-F77DF5C5DA15}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFF4E3C3-5723-4C72-A526-55D750275B60}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{025AB5CD-E76C-44A2-B242-E9FE70EE6D55}"/>
   </bookViews>
@@ -34,15 +34,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="45">
   <si>
     <t xml:space="preserve">Titulo </t>
   </si>
   <si>
     <t xml:space="preserve">Historia de usuario </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Asignación </t>
   </si>
   <si>
     <t xml:space="preserve">Pasos a reproducir </t>
@@ -157,6 +154,36 @@
   </si>
   <si>
     <t>Al dirigirnos en el apartado URL en {{username}} ingresamos un valor numérico entero, tiene que comparar con el usermane existente para que se proceda con la petición haciendo que este lo tome como válido procediendo a dar clic en send y que mande un status code 200 OK.</t>
+  </si>
+  <si>
+    <t>Requisitos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Estado </t>
+  </si>
+  <si>
+    <t>In progress</t>
+  </si>
+  <si>
+    <t>Identificador</t>
+  </si>
+  <si>
+    <t>CP1_Bug1</t>
+  </si>
+  <si>
+    <t>CP2_Bug2</t>
+  </si>
+  <si>
+    <t>User_Bug5</t>
+  </si>
+  <si>
+    <t>CP4_Bug4</t>
+  </si>
+  <si>
+    <t>CP3_Bug3</t>
+  </si>
+  <si>
+    <t>Tener acceso a los swaggers, tener la herramienta postman</t>
   </si>
 </sst>
 </file>
@@ -572,9 +599,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B16F273-31EA-4199-8111-E5898421FD0E}">
-  <dimension ref="B2:J10"/>
+  <dimension ref="A2:K10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
       <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
@@ -582,7 +609,7 @@
   <cols>
     <col min="2" max="2" width="21.88671875" customWidth="1"/>
     <col min="3" max="3" width="16.21875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.77734375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.6640625" customWidth="1"/>
     <col min="5" max="5" width="34.6640625" customWidth="1"/>
     <col min="6" max="6" width="39.77734375" customWidth="1"/>
     <col min="7" max="7" width="42.77734375" customWidth="1"/>
@@ -591,7 +618,10 @@
     <col min="10" max="10" width="8.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A2" s="4" t="s">
+        <v>38</v>
+      </c>
       <c r="B2" s="4" t="s">
         <v>0</v>
       </c>
@@ -599,28 +629,31 @@
         <v>1</v>
       </c>
       <c r="D2" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="E2" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="F2" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="G2" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="4" t="s">
+      <c r="H2" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="H2" s="4" t="s">
+      <c r="I2" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="I2" s="4" t="s">
+      <c r="J2" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="J2" s="4" t="s">
-        <v>8</v>
+      <c r="K2" s="4" t="s">
+        <v>36</v>
       </c>
     </row>
-    <row r="3" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
@@ -631,142 +664,182 @@
       <c r="I3" s="1"/>
       <c r="J3" s="1"/>
     </row>
-    <row r="4" spans="2:10" ht="165.6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" ht="165.6" x14ac:dyDescent="0.3">
+      <c r="A4" s="5" t="s">
+        <v>39</v>
+      </c>
       <c r="B4" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="G4" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="H4" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="I4" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="J4" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="K4" s="5" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" ht="124.2" x14ac:dyDescent="0.3">
+      <c r="A5" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="B5" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="C5" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="E5" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="D4" s="5"/>
-      <c r="E4" s="2" t="s">
+      <c r="F5" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="F4" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="G4" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="H4" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="I4" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="J4" s="5" t="s">
-        <v>11</v>
+      <c r="G5" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="H5" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="I5" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="J5" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="K5" s="5" t="s">
+        <v>37</v>
       </c>
     </row>
-    <row r="5" spans="2:10" ht="124.2" x14ac:dyDescent="0.3">
-      <c r="B5" s="5" t="s">
+    <row r="6" spans="1:11" ht="138" x14ac:dyDescent="0.3">
+      <c r="A6" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C5" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="D5" s="5"/>
-      <c r="E5" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="F5" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="G5" s="5" t="s">
+      <c r="D6" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="F6" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="G6" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="H5" s="5" t="s">
+      <c r="H6" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="I5" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="J5" s="5" t="s">
-        <v>11</v>
+      <c r="I6" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="J6" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="K6" s="5" t="s">
+        <v>37</v>
       </c>
     </row>
-    <row r="6" spans="2:10" ht="138" x14ac:dyDescent="0.3">
-      <c r="B6" s="5" t="s">
+    <row r="7" spans="1:11" ht="138" x14ac:dyDescent="0.3">
+      <c r="A7" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="C7" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="D6" s="5"/>
-      <c r="E6" s="2" t="s">
+      <c r="D7" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="E7" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="F6" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="G6" s="5" t="s">
+      <c r="F7" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="G7" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="H7" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="H6" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="I6" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="J6" s="5" t="s">
-        <v>11</v>
+      <c r="I7" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="J7" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="K7" s="5" t="s">
+        <v>37</v>
       </c>
     </row>
-    <row r="7" spans="2:10" ht="138" x14ac:dyDescent="0.3">
-      <c r="B7" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="C7" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="D7" s="5"/>
-      <c r="E7" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="F7" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="G7" s="5" t="s">
+    <row r="8" spans="1:11" ht="124.2" x14ac:dyDescent="0.3">
+      <c r="A8" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="C8" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="H7" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="I7" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="J7" s="5" t="s">
-        <v>11</v>
+      <c r="D8" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="F8" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="G8" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="H8" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="I8" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="J8" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="K8" s="5" t="s">
+        <v>37</v>
       </c>
     </row>
-    <row r="8" spans="2:10" ht="124.2" x14ac:dyDescent="0.3">
-      <c r="B8" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="C8" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="D8" s="5"/>
-      <c r="E8" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="F8" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="G8" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="H8" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="I8" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="J8" s="5" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="9" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B9" s="5"/>
       <c r="C9" s="5"/>
       <c r="D9" s="5"/>
@@ -777,7 +850,7 @@
       <c r="I9" s="5"/>
       <c r="J9" s="5"/>
     </row>
-    <row r="10" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B10" s="5"/>
       <c r="C10" s="5"/>
       <c r="D10" s="5"/>

</xml_diff>

<commit_message>
Modified test cases according to feedback
</commit_message>
<xml_diff>
--- a/DesignAndExecution/Bugs PetStore.xlsx
+++ b/DesignAndExecution/Bugs PetStore.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\drago\OneDrive\Escritorio\Punto Singular\Proyecto Plan de Pruebas\Pruebas Esploratorias\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\drago\Automatizacion\QAproyecAutom\DesignAndExecution\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFF4E3C3-5723-4C72-A526-55D750275B60}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D80FBDC0-FED6-4F51-91E8-530F3F5025BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{025AB5CD-E76C-44A2-B242-E9FE70EE6D55}"/>
   </bookViews>
@@ -601,7 +601,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B16F273-31EA-4199-8111-E5898421FD0E}">
   <dimension ref="A2:K10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>

</xml_diff>